<commit_message>
Updated SQM with Test report and release note links
</commit_message>
<xml_diff>
--- a/docs/design/GC2115/R0V32/SW-SQM-GC2115-R1.xlsx
+++ b/docs/design/GC2115/R0V32/SW-SQM-GC2115-R1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BBCE0F-C45E-4972-80C2-67B6CA8B89B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{B78389F3-9353-4BAE-BA08-6E2FC0694597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5804160-E6D8-4C2D-82D1-623488E68224}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="137">
   <si>
     <t>SEDEMAC</t>
   </si>
@@ -694,10 +694,6 @@
     <t>MODBUS MAP has been attched  in the test report</t>
   </si>
   <si>
-    <t xml:space="preserve">Reviewed by
-Rahul Hage[SYSE] </t>
-  </si>
-  <si>
     <t>Confluence Page</t>
   </si>
   <si>
@@ -769,6 +765,13 @@
   </si>
   <si>
     <t>Software Quality Metric For : GC2115 R1.01 (Firmware : R0.32)</t>
+  </si>
+  <si>
+    <t>Ramachandran S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODBUS map is reviewed by
+Rahul Hage[SYSE] </t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1565,7 @@
   <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="G33" sqref="G33:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1595,7 @@
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D1" s="52"/>
       <c r="E1" s="43" t="s">
@@ -1600,7 +1603,7 @@
       </c>
       <c r="F1" s="44"/>
       <c r="G1" s="60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H1" s="60"/>
       <c r="N1" t="s">
@@ -1617,7 +1620,7 @@
       </c>
       <c r="F2" s="44"/>
       <c r="G2" s="63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H2" s="63"/>
       <c r="L2" t="s">
@@ -1671,7 +1674,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="61" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="61"/>
       <c r="E4" s="61"/>
@@ -1738,7 +1741,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="61" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" s="61"/>
       <c r="E6" s="61"/>
@@ -1764,7 +1767,7 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="61" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="D7" s="61"/>
       <c r="E7" s="61"/>
@@ -1778,7 +1781,7 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D8" s="62"/>
       <c r="E8" s="62"/>
@@ -1795,14 +1798,14 @@
         <v>37</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="10" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="10"/>
@@ -1814,14 +1817,14 @@
         <v>38</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E10" s="73"/>
       <c r="F10" s="10" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="10"/>
@@ -1833,14 +1836,14 @@
         <v>39</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="10" t="s">
         <v>39</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="10"/>
@@ -1852,14 +1855,14 @@
         <v>40</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="10" t="s">
         <v>40</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="10"/>
@@ -1915,7 +1918,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H15" s="25"/>
       <c r="R15" s="13" t="s">
@@ -2041,7 +2044,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H21" s="20"/>
       <c r="R21" s="12" t="s">
@@ -2133,7 +2136,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H25" s="20"/>
       <c r="R25" s="12" t="s">
@@ -2249,7 +2252,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H30" s="16"/>
       <c r="R30" s="12" t="s">
@@ -2287,12 +2290,12 @@
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3">
         <f>IF(D32="Yes",1,IF(D32="Not Applicable",0.5,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="33" t="s">
         <v>111</v>
@@ -2311,15 +2314,15 @@
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3">
         <f>IF(AND(D32="Yes",D33="Yes"),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="H33" s="21"/>
       <c r="R33" s="12" t="s">
@@ -2433,7 +2436,7 @@
         <v>5</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H38" s="21"/>
       <c r="R38" s="12" t="s">
@@ -2449,15 +2452,14 @@
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3">
-        <f>IF(D39="Yes",5,0)</f>
         <v>5</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H39" s="21"/>
       <c r="R39" s="12" t="s">
@@ -2505,7 +2507,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H41" s="21"/>
       <c r="R41" s="12" t="s">
@@ -2573,7 +2575,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H44" s="21"/>
       <c r="R44" s="12" t="s">
@@ -2773,7 +2775,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H53" s="25"/>
       <c r="R53" s="12" t="s">
@@ -2805,7 +2807,7 @@
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F55" s="3">
         <f>F16+SUM(F19:F54)-F42-F43</f>
-        <v>85.2</v>
+        <v>83.2</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
@@ -2814,7 +2816,7 @@
       </c>
       <c r="D58" s="4">
         <f>F55</f>
-        <v>85.2</v>
+        <v>83.2</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -3024,26 +3026,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1368c656-b5be-4b92-a170-f03a090da0eb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="09c4be65-2cf9-46da-869c-d5826f262cb1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100854852AB1FCCB343B38344B0B41716E7" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f3072bb31fb469f1da3162ac9bfbed5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1368c656-b5be-4b92-a170-f03a090da0eb" xmlns:ns3="09c4be65-2cf9-46da-869c-d5826f262cb1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b182ede65aa816d91ef00987d518e42" ns2:_="" ns3:_="">
     <xsd:import namespace="1368c656-b5be-4b92-a170-f03a090da0eb"/>
@@ -3286,26 +3268,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB296EE7-E205-4D20-97DE-474F1D44B89F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1368c656-b5be-4b92-a170-f03a090da0eb"/>
-    <ds:schemaRef ds:uri="09c4be65-2cf9-46da-869c-d5826f262cb1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1368c656-b5be-4b92-a170-f03a090da0eb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="09c4be65-2cf9-46da-869c-d5826f262cb1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C9098F7-9747-4B0C-A7F4-326F37B81062}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58522EE4-9543-446C-870D-236E82CB8943}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3322,4 +3305,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB296EE7-E205-4D20-97DE-474F1D44B89F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1368c656-b5be-4b92-a170-f03a090da0eb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="09c4be65-2cf9-46da-869c-d5826f262cb1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C9098F7-9747-4B0C-A7F4-326F37B81062}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>